<commit_message>
seems ok, need to be checked
</commit_message>
<xml_diff>
--- a/resources/Cold.xlsx
+++ b/resources/Cold.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,15 +448,15 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="C4" sqref="C4:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,10 +472,10 @@
         <v>40909</v>
       </c>
       <c r="C2" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,10 +483,10 @@
         <v>40909.041666666664</v>
       </c>
       <c r="C3" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -494,10 +494,10 @@
         <v>40909.083333333336</v>
       </c>
       <c r="C4" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -505,10 +505,10 @@
         <v>40909.125</v>
       </c>
       <c r="C5" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -516,10 +516,10 @@
         <v>40909.166666666664</v>
       </c>
       <c r="C6" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -527,10 +527,10 @@
         <v>40909.208333333336</v>
       </c>
       <c r="C7" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -538,10 +538,10 @@
         <v>40909.25</v>
       </c>
       <c r="C8" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -549,10 +549,10 @@
         <v>40909.291666666664</v>
       </c>
       <c r="C9" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -560,10 +560,10 @@
         <v>40909.333333333336</v>
       </c>
       <c r="C10" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -571,7 +571,7 @@
         <v>40909.375</v>
       </c>
       <c r="C11" s="2">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>